<commit_message>
login using the username/password extracted from excel file
</commit_message>
<xml_diff>
--- a/src/test/java/tutorial/testData/TestData.xlsx
+++ b/src/test/java/tutorial/testData/TestData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsqa\src\test\java\tutorial\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8844"/>
+    <workbookView windowHeight="8844" windowWidth="23040" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -45,12 +45,16 @@
   </si>
   <si>
     <t>test123</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,17 +90,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -113,10 +117,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -151,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -203,7 +207,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -314,21 +318,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -345,7 +349,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -397,14 +401,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -414,10 +418,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.33203125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.77734375" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -444,9 +448,12 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>